<commit_message>
Correction readme clavier et update MAN
</commit_message>
<xml_diff>
--- a/Documentation/Manuel_Technique/Exemple_EvaluationCouts.xlsx
+++ b/Documentation/Manuel_Technique/Exemple_EvaluationCouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Documentation\Manuel_Technique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D196FC7E-A1E3-4AE0-BF6A-661261586A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2BA0F3-C2BC-4765-B49C-84A01A52AA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>https://www.pishop.ca/product/raspberry-pi-4-model-b-4gb/</t>
+  </si>
+  <si>
+    <t>En pack de 5, 150 pour les PCB et 50 pour le transport</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +213,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -380,7 +389,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -435,6 +444,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Accent3" xfId="7" builtinId="37"/>
@@ -759,7 +769,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +811,9 @@
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="30" t="s">
+        <v>23</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
@@ -809,14 +821,14 @@
         <v>30</v>
       </c>
       <c r="E2" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="9">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G2" s="16">
         <f>(D2*E2)+F2</f>
-        <v>200</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -966,7 +978,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="17">
         <f>SUM(G2:G15)</f>
-        <v>293.57</v>
+        <v>133.57</v>
       </c>
     </row>
     <row r="18" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -977,7 +989,7 @@
       <c r="F18" s="26"/>
       <c r="G18" s="18">
         <f>G17*0.15</f>
-        <v>44.035499999999999</v>
+        <v>20.035499999999999</v>
       </c>
     </row>
     <row r="19" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -988,7 +1000,7 @@
       <c r="F19" s="29"/>
       <c r="G19" s="16">
         <f>SUM(G17:G18)</f>
-        <v>337.60550000000001</v>
+        <v>153.60550000000001</v>
       </c>
     </row>
     <row r="20" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1062,6 +1074,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DDF7F2FCC1D2C469E7882E767051E21" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fdb502a7565e043baea1e7044cb52160">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de9a939f-7971-4532-9b84-38cbdf21fdbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87cf97e6ee09886aa213502e86bb7644" ns2:_="">
     <xsd:import namespace="de9a939f-7971-4532-9b84-38cbdf21fdbe"/>
@@ -1205,22 +1232,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{933EE957-C7CB-4D6D-82A9-7153ECCB8F4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="59f032a8-2326-4110-a897-48ad6ab7eae4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDB945AF-1AEA-41ED-B8A1-BD2374DCFC92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1236,22 +1266,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{933EE957-C7CB-4D6D-82A9-7153ECCB8F4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="59f032a8-2326-4110-a897-48ad6ab7eae4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update MAN et ajout stl equerre
</commit_message>
<xml_diff>
--- a/Documentation/Manuel_Technique/Exemple_EvaluationCouts.xlsx
+++ b/Documentation/Manuel_Technique/Exemple_EvaluationCouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Documentation\Manuel_Technique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2BA0F3-C2BC-4765-B49C-84A01A52AA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554EE80F-924D-4379-BE13-3C284FD88B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Sous-total</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Nom et numéro de la pièce</t>
   </si>
   <si>
-    <t>Transport</t>
-  </si>
-  <si>
     <t>Dans l'évaluation des coûts, ne pas oublier:</t>
   </si>
   <si>
@@ -108,7 +102,52 @@
     <t>https://www.pishop.ca/product/raspberry-pi-4-model-b-4gb/</t>
   </si>
   <si>
-    <t>En pack de 5, 150 pour les PCB et 50 pour le transport</t>
+    <t>https://caseplace.ca/products/pelican-1500-case</t>
+  </si>
+  <si>
+    <t>Case pelican 1500</t>
+  </si>
+  <si>
+    <t>Esp32 c3 devkit-02</t>
+  </si>
+  <si>
+    <t>3 esp32</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Espressif-Systems/ESP32-C3-DevKitC-02?qs=stqOd1AaK7%2F1Q62ysr4CMA%3D%3D</t>
+  </si>
+  <si>
+    <t>Plastique gravé sur mesure</t>
+  </si>
+  <si>
+    <t>La mallette pour contenir l'énigme</t>
+  </si>
+  <si>
+    <t>PCB sur mesure en pack de 5, 95.19$/5</t>
+  </si>
+  <si>
+    <t>Voir pdf de commision</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/-/fr/GeeekPi-Raspberry-moniteur-portable-gratuit/dp/B0CPLYD5GD?th=1</t>
+  </si>
+  <si>
+    <t>GeeekPi 10.1 Inch LCD Screen for Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Mini écran pour l'affichage des énigmes</t>
+  </si>
+  <si>
+    <t>Prix Total</t>
+  </si>
+  <si>
+    <t>Doubleur usb</t>
+  </si>
+  <si>
+    <t>Doubleur usb pour alimenter PCB et Écran</t>
+  </si>
+  <si>
+    <t>Lien amazon</t>
   </si>
 </sst>
 </file>
@@ -118,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,13 +216,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF0F1111"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -220,8 +252,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,11 +301,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -277,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -345,9 +386,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -360,26 +399,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,67 +413,58 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="7" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Accent3" xfId="7" builtinId="37"/>
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -768,253 +785,297 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="3" max="3" width="105.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>4</v>
+      <c r="F1" s="24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7">
+        <v>19.04</v>
+      </c>
+      <c r="E2" s="25">
+        <v>1</v>
+      </c>
+      <c r="F2" s="28">
+        <f>D2*E2</f>
+        <v>19.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7">
+        <v>76.45</v>
+      </c>
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="F3" s="28">
+        <f t="shared" ref="F3:F8" si="0">D3*E3</f>
+        <v>76.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7">
+        <v>223.95</v>
+      </c>
+      <c r="E4" s="25">
+        <v>1</v>
+      </c>
+      <c r="F4" s="28">
+        <f t="shared" si="0"/>
+        <v>223.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="25">
+        <v>3</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7">
+        <v>330</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1</v>
+      </c>
+      <c r="F6" s="28">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="9">
+      <c r="D7" s="7">
+        <v>89.9</v>
+      </c>
+      <c r="E7" s="25">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
-        <v>10</v>
-      </c>
-      <c r="G2" s="16">
-        <f>(D2*E2)+F2</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="8">
-        <v>76.45</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="F7" s="28">
+        <f t="shared" si="0"/>
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="7">
+        <v>9</v>
+      </c>
+      <c r="E8" s="26">
         <v>1</v>
       </c>
-      <c r="F3" s="9">
-        <v>17.12</v>
-      </c>
-      <c r="G3" s="16">
-        <f t="shared" ref="G3" si="0">(D3 * E3) + F3</f>
-        <v>93.570000000000007</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="28">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="28"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="16"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="21" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="12">
+        <f>SUM(D2:D15)</f>
+        <v>760.34</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="17">
-        <f>SUM(G2:G15)</f>
-        <v>133.57</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="24" t="s">
+      <c r="E18" s="20"/>
+      <c r="F18" s="13">
+        <f>F17*0.15</f>
+        <v>114.051</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="18">
-        <f>G17*0.15</f>
-        <v>20.035499999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="16">
-        <f>SUM(G17:G18)</f>
-        <v>153.60550000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="11">
+        <f>SUM(F17:F18)</f>
+        <v>874.39100000000008</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{3BDDC1A7-7120-4843-A415-CF7B402312D0}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{F7962BBD-31DC-40E9-B7A5-B14DFC489B7A}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{11E95A54-44D3-4FC8-A896-E24721B414A8}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{30E4ED57-763F-48EF-8AA3-5C8608FADA9B}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{CDDC0493-472A-4D7C-84C7-3737CFA7E3CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1030,42 +1091,42 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1074,21 +1135,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DDF7F2FCC1D2C469E7882E767051E21" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fdb502a7565e043baea1e7044cb52160">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de9a939f-7971-4532-9b84-38cbdf21fdbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87cf97e6ee09886aa213502e86bb7644" ns2:_="">
     <xsd:import namespace="de9a939f-7971-4532-9b84-38cbdf21fdbe"/>
@@ -1232,10 +1278,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDB945AF-1AEA-41ED-B8A1-BD2374DCFC92}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="de9a939f-7971-4532-9b84-38cbdf21fdbe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1251,19 +1322,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDB945AF-1AEA-41ED-B8A1-BD2374DCFC92}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="de9a939f-7971-4532-9b84-38cbdf21fdbe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MAN fini sans correction et formatage
</commit_message>
<xml_diff>
--- a/Documentation/Manuel_Technique/Exemple_EvaluationCouts.xlsx
+++ b/Documentation/Manuel_Technique/Exemple_EvaluationCouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Documentation\Manuel_Technique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554EE80F-924D-4379-BE13-3C284FD88B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB66AAB0-801C-4929-AB15-C5F899EFC607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>Lien amazon</t>
+  </si>
+  <si>
+    <t>Bouton lumineux en pack de 5, 21$/5</t>
+  </si>
+  <si>
+    <t>Bouton lumineux</t>
+  </si>
+  <si>
+    <t>Logarithmic Slide Potentiometer</t>
+  </si>
+  <si>
+    <t>Oiyagai 20Pcs Amplifier Terminal Connector</t>
+  </si>
+  <si>
+    <t>Bornes bannes en pack de 20, 15.50$/20</t>
+  </si>
+  <si>
+    <t>Potentiomètre glissant en pack de 5, 24.40$/5</t>
   </si>
 </sst>
 </file>
@@ -157,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,12 +265,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -260,11 +272,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -414,7 +425,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -437,7 +448,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,13 +471,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -783,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,7 +809,7 @@
     <col min="7" max="7" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -813,18 +822,18 @@
       <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -833,15 +842,15 @@
       <c r="D2" s="7">
         <v>19.04</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="17">
         <v>1</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="20">
         <f>D2*E2</f>
         <v>19.04</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>18</v>
       </c>
@@ -854,15 +863,15 @@
       <c r="D3" s="7">
         <v>76.45</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="17">
         <v>1</v>
       </c>
-      <c r="F3" s="28">
-        <f t="shared" ref="F3:F8" si="0">D3*E3</f>
+      <c r="F3" s="20">
+        <f t="shared" ref="F3:F11" si="0">D3*E3</f>
         <v>76.45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -875,15 +884,15 @@
       <c r="D4" s="7">
         <v>223.95</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="17">
         <v>1</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="20">
         <f t="shared" si="0"/>
         <v>223.95</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -896,37 +905,37 @@
       <c r="D5" s="7">
         <v>12</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="17">
         <v>3</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="20">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="7">
         <v>330</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="17">
         <v>1</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="20">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -939,15 +948,15 @@
       <c r="D7" s="7">
         <v>89.9</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="17">
         <v>1</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="20">
         <f t="shared" si="0"/>
         <v>89.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -960,104 +969,142 @@
       <c r="D8" s="7">
         <v>9</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="18">
         <v>1</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="28"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4.2</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4.88</v>
+      </c>
+      <c r="E10" s="17">
+        <v>3</v>
+      </c>
+      <c r="F10" s="20">
+        <f t="shared" si="0"/>
+        <v>14.64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="E11" s="17">
+        <v>8</v>
+      </c>
+      <c r="F11" s="20">
+        <f t="shared" si="0"/>
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="27"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="17"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="27"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="17"/>
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="27"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="17"/>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="27"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="17"/>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="12">
         <f>SUM(D2:D15)</f>
-        <v>760.34</v>
+        <v>770.2</v>
       </c>
     </row>
     <row r="18" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="13">
         <f>F17*0.15</f>
-        <v>114.051</v>
+        <v>115.53</v>
       </c>
     </row>
     <row r="19" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="22"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="11">
         <f>SUM(F17:F18)</f>
-        <v>874.39100000000008</v>
+        <v>885.73</v>
       </c>
     </row>
     <row r="20" spans="4:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1073,9 +1120,12 @@
     <hyperlink ref="C5" r:id="rId3" xr:uid="{11E95A54-44D3-4FC8-A896-E24721B414A8}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{30E4ED57-763F-48EF-8AA3-5C8608FADA9B}"/>
     <hyperlink ref="C8" r:id="rId5" xr:uid="{CDDC0493-472A-4D7C-84C7-3737CFA7E3CB}"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://www.amazon.ca/EG-STARTS-Illuminated-Buttons-Operated/dp/B01M7PNCO9?crid=3CVHLC58BHKFS&amp;dib=eyJ2IjoiMSJ9.XHLNCEukSTJ_YW3CSeiwVLZ0w8qC02zpScstbmpYmL-26dh49nC7Stwk-_wSUfpaNo9j79LlUsUTm7lt4mYhyShMJ4ZXyU58ViOk8AKLN9VNmF_CiKpoID5EanPPF8_VZugoqUyB-VNEJVGqhPDqYpxBHx_iKeRUOPOkFO84TqM3e630_d2RLyvNPRQk_eGGAacxe5xORhR1scuZypotN8pSDFYjJwliwqYeu90CiOnfVyQF8fM7INVmViEWtVE4UKZK5t_t-cmHocLw2ylJXQKj07LExR2mFRM1COqZw8s.IdYCX76yLHe8sg3S8jW3oTOKf4w_KSt3672Okit5vzU&amp;dib_tag=se&amp;keywords=bouton+lumineux&amp;qid=1745327004&amp;sprefix=bouton+lum%2Caps%2C98&amp;sr=8-7" xr:uid="{E0F27853-41B0-4792-9A18-8CD6C73D348B}"/>
+    <hyperlink ref="C10" r:id="rId7" display="https://www.amazon.ca/DAOKI-Logarithmic-Potentiometer-Arduino-Electronic/dp/B08SLPV4VD?crid=38N9GBJ03GKC4&amp;dib=eyJ2IjoiMSJ9.c-dP0cG3lrrWUnfE5mJI7gV88z7m_oaCPIu8ssmlQlrXxwaxepMKl-86tptvfDFKjMXpCn4rLfBk1OmRHXGccKIBgrrL4tVqPzSFO_9ew7Axty9IWEhxGqkh-gkTwyiWHczjcLBVrGEsZvJ1HLSqpSNb4u4_cGPaagDTEN2lsQF8aBREdxkOndtb4YekNZHdUa2Cqnz7HdcxaNSVtT0APVnMktfq2-b_lRypcIpSQFA.IztW89hD37MpgWDtjcd_NqEy9fczQ3qTymYS0X1fPVM&amp;dib_tag=se&amp;keywords=potentiom%C3%A8tre+glissant&amp;qid=1745327147&amp;sprefix=potentiom%C3%A8tre+glissant%2Caps%2C70&amp;sr=8-7" xr:uid="{1B5D632D-03E8-4DAE-9641-02AF0B01DB83}"/>
+    <hyperlink ref="C11" r:id="rId8" display="https://www.amazon.ca/Oiyagai-Amplifier-Terminal-Connector-Binding/dp/B07D3MMBJH?crid=3PUPCH85601FJ&amp;dib=eyJ2IjoiMSJ9.uV8yQ4336UxscpdZEhd8nIt_EXyn8wK96F1xmsUbSGqduc9IhzdI5CAg1yQbo6S8bAbCmRVywmwmRi_ReTpY8wXMi5n-OlSmwGjOtfb69xh9BH_xuEHLcJsaNyTg0RtbdC-qvDK1VNYTVRX-jlJtpwFQz81NcekGo9J_HA_4Tge4kUJfj2gCxiCEIK1Gd0RYtlzGNQUQcOlGE2AJCF1tbojS_TM4GGCc0QJfkB-YpndrX_1sS314bfmHY8tJJPxhhgDOHBk2ppRcyf3C1OymKDabdIteC7lpREsxuS7GOEE.b4ikTgT6AhpP070V7Ug5e7iCZWUfJO7Yd6TNbg-DB_o&amp;dib_tag=se&amp;keywords=borne+banane&amp;qid=1745327282&amp;sprefix=borne+banane%2Caps%2C70&amp;sr=8-54" xr:uid="{4A1A319E-4CF8-49BE-8A12-B4ACABFA8996}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1135,6 +1185,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DDF7F2FCC1D2C469E7882E767051E21" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fdb502a7565e043baea1e7044cb52160">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de9a939f-7971-4532-9b84-38cbdf21fdbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87cf97e6ee09886aa213502e86bb7644" ns2:_="">
     <xsd:import namespace="de9a939f-7971-4532-9b84-38cbdf21fdbe"/>
@@ -1278,22 +1343,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{933EE957-C7CB-4D6D-82A9-7153ECCB8F4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="59f032a8-2326-4110-a897-48ad6ab7eae4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDB945AF-1AEA-41ED-B8A1-BD2374DCFC92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1309,22 +1377,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{933EE957-C7CB-4D6D-82A9-7153ECCB8F4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="59f032a8-2326-4110-a897-48ad6ab7eae4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>